<commit_message>
avance hasta 29 de agosto de 2020
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Documents\Github\PracticasIntermedias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Moraza\PracticasIntermedias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2A94177-F431-45BB-BE9F-2F668BFE9F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA816E69-8E6D-47DC-ADE1-290ECA36FF89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,9 +173,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -184,6 +180,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,48 +496,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72354E02-C4E5-4CFE-AC76-15CE50841123}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,7 +556,7 @@
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -576,165 +575,165 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>